<commit_message>
fix importing vcfs + fix emx/vcf files
</commit_message>
<xml_diff>
--- a/molgenis-app/src/test/resources/test_annotate_computed.xlsx
+++ b/molgenis-app/src/test/resources/test_annotate_computed.xlsx
@@ -1,10 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25317"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26024"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="5520" yWindow="2320" windowWidth="22980" windowHeight="12560" tabRatio="500" activeTab="2"/>
+    <workbookView xWindow="-34780" yWindow="-4240" windowWidth="25040" windowHeight="14960" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="attributes" sheetId="2" r:id="rId1"/>
@@ -1476,8 +1476,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1661,7 +1661,7 @@
         <v>27</v>
       </c>
       <c r="F9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="K9" t="b">
         <v>1</v>
@@ -1871,7 +1871,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E420"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>

</xml_diff>